<commit_message>
cleaned data and updated
</commit_message>
<xml_diff>
--- a/responses/s2_simulation_tools.xlsx
+++ b/responses/s2_simulation_tools.xlsx
@@ -1,22 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au513437_uni_au_dk/Documents/PhD/papers/phd_project/urdf_files/questionnaire/responses/final/csv_completed_responses/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniella\Desktop\git_repos\urdf_survey_material\responses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{1755FB2F-68A5-4321-89D2-3C6FAA0FD034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C7C68C-6BAF-44C8-9D9D-EFC3F794CD0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="s2_simulation_tools" sheetId="1" r:id="rId1"/>
     <sheet name="classification" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -929,7 +942,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1770,7 +1783,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:B496"/>
   <sheetViews>
     <sheetView topLeftCell="A451" workbookViewId="0">
@@ -5006,11 +5019,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L495"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5075,6 +5088,10 @@
         <f>COUNTIF(F2:I496,"*Pinocchio*")</f>
         <v>2</v>
       </c>
+      <c r="L2">
+        <f>K2/K22*100</f>
+        <v>1.3245033112582782</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -5181,6 +5198,10 @@
         <f>COUNTIF(F2:I496,"*Meshcat*")</f>
         <v>4</v>
       </c>
+      <c r="L7">
+        <f>K7/K22*100</f>
+        <v>2.6490066225165565</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -5198,6 +5219,10 @@
         <f>COUNTIF(F2:I496,"*Julia*")</f>
         <v>2</v>
       </c>
+      <c r="L8">
+        <f>K8/K22*100</f>
+        <v>1.3245033112582782</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -5220,6 +5245,10 @@
         <f>COUNTIF(F2:I496,"*Godot*")</f>
         <v>1</v>
       </c>
+      <c r="L9">
+        <f>K9/K22*100</f>
+        <v>0.66225165562913912</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -5266,6 +5295,10 @@
         <f>COUNTIF(F2:I496,"*Foxglove*")</f>
         <v>1</v>
       </c>
+      <c r="L11">
+        <f>K11/K22*100</f>
+        <v>0.66225165562913912</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -5283,6 +5316,10 @@
         <f>COUNTIF(F2:I496,"*Blender*")</f>
         <v>4</v>
       </c>
+      <c r="L12">
+        <f>K12/K22*100</f>
+        <v>2.6490066225165565</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -5299,6 +5336,10 @@
       <c r="K13">
         <f>COUNTIF(F2:I496,"*20-sim*")</f>
         <v>1</v>
+      </c>
+      <c r="L13">
+        <f>K13/K22*100</f>
+        <v>0.66225165562913912</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -5346,6 +5387,10 @@
         <f>COUNTIF(F2:I496,"*AGX Dynamics*")</f>
         <v>3</v>
       </c>
+      <c r="L16">
+        <f>K16/K22*100</f>
+        <v>1.9867549668874174</v>
+      </c>
     </row>
     <row r="17" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E17" s="3"/>
@@ -5356,6 +5401,10 @@
         <f>COUNTIF(F2:I496,"*Modelica*")</f>
         <v>2</v>
       </c>
+      <c r="L17">
+        <f>K17/K22*100</f>
+        <v>1.3245033112582782</v>
+      </c>
     </row>
     <row r="18" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E18" s="3"/>
@@ -7485,7 +7534,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:I495">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:I495" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>$J$2:$J$21</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>